<commit_message>
Online_Shop für Gruppe FIAE B
</commit_message>
<xml_diff>
--- a/Online_Shop.Projekt_FIAE_B.xlsx
+++ b/Online_Shop.Projekt_FIAE_B.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t xml:space="preserve">Beispiel: Funktionsorientierter Projektstrukturplan</t>
   </si>
@@ -46,94 +46,49 @@
     <t xml:space="preserve">Arbeitspaket</t>
   </si>
   <si>
-    <t xml:space="preserve">1.2.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Datenbank erstellen</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Produkte kategorisieren</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1.2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Produkte erfassen</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Produktfotos erstellen</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1.4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Produktfotos bearbeiten</t>
   </si>
   <si>
-    <t xml:space="preserve">1.2.2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Template auswählen</t>
   </si>
   <si>
-    <t xml:space="preserve">1.2.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Seitenstruktur einrichten</t>
   </si>
   <si>
-    <t xml:space="preserve">1.2.4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Datenbank einbinden</t>
   </si>
   <si>
     <t xml:space="preserve">Zahlungsdienste einbinden</t>
   </si>
   <si>
-    <t xml:space="preserve">1.2.6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bewertungssystem anpassen</t>
   </si>
   <si>
-    <t xml:space="preserve">1.3.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Handbücher erstellen</t>
   </si>
   <si>
-    <t xml:space="preserve">1.3.2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tests</t>
   </si>
   <si>
-    <t xml:space="preserve">1.2.7</t>
-  </si>
-  <si>
     <t xml:space="preserve">Korrekturen</t>
   </si>
   <si>
-    <t xml:space="preserve">1.3.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Auftraggeber-Präsentation</t>
   </si>
   <si>
-    <t xml:space="preserve">1.2.8</t>
-  </si>
-  <si>
     <t xml:space="preserve">eventuelle Korrekturen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.9</t>
   </si>
   <si>
     <t xml:space="preserve">Onlinestellung</t>
@@ -477,7 +432,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8171640" y="325080"/>
+          <a:off x="8180280" y="325080"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -501,13 +456,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>885240</xdr:colOff>
+      <xdr:colOff>885600</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>901800</xdr:colOff>
+      <xdr:colOff>902160</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>154440</xdr:rowOff>
     </xdr:to>
@@ -518,8 +473,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5430600" y="479520"/>
-          <a:ext cx="5483880" cy="0"/>
+          <a:off x="5436000" y="479520"/>
+          <a:ext cx="5491800" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -559,7 +514,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5452560" y="488160"/>
+          <a:off x="5457600" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -600,7 +555,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5457600" y="488160"/>
+          <a:off x="5464080" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -641,7 +596,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8191440" y="488160"/>
+          <a:off x="8201520" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -682,7 +637,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10924560" y="488160"/>
+          <a:off x="10938600" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -723,7 +678,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5457600" y="1122120"/>
+          <a:off x="5464080" y="1122120"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -764,7 +719,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8191440" y="1122120"/>
+          <a:off x="8201520" y="1122120"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -805,7 +760,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10924920" y="1121760"/>
+          <a:off x="10938960" y="1121760"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -836,11 +791,11 @@
   </sheetPr>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I29:I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.94921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.77"/>
   </cols>
@@ -981,161 +936,129 @@
       <c r="D25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="A27" s="10"/>
       <c r="B27" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="A28" s="10"/>
       <c r="B28" s="11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
-        <v>14</v>
-      </c>
+      <c r="A29" s="10"/>
       <c r="B29" s="11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="A30" s="10"/>
       <c r="B30" s="11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10" t="s">
-        <v>18</v>
-      </c>
+      <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="A33" s="10"/>
       <c r="B33" s="11" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="A34" s="10"/>
       <c r="B34" s="11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10" t="s">
-        <v>25</v>
-      </c>
+      <c r="A35" s="10"/>
       <c r="B35" s="11" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="s">
-        <v>27</v>
-      </c>
+      <c r="A36" s="10"/>
       <c r="B36" s="11" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="s">
-        <v>29</v>
-      </c>
+      <c r="A37" s="10"/>
       <c r="B37" s="11" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="s">
-        <v>31</v>
-      </c>
+      <c r="A38" s="10"/>
       <c r="B38" s="11" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="s">
-        <v>33</v>
-      </c>
+      <c r="A39" s="10"/>
       <c r="B39" s="11" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10" t="s">
-        <v>35</v>
-      </c>
+      <c r="A40" s="10"/>
       <c r="B40" s="11" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12" t="s">
-        <v>37</v>
-      </c>
+      <c r="A41" s="12"/>
       <c r="B41" s="13" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>

</xml_diff>